<commit_message>
tests are is separate files in order to support parallelization. added subfolder to test for better organization and script --recursive, so mocha can find from subfolders.
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Automation first steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC520AB-ACF5-4CC0-825C-01BEB320FF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D69F77-984E-4CDF-86C3-91CE66257485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
-    <t>Test cases:</t>
-  </si>
-  <si>
     <t>Goal</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   <si>
     <t>1. Inventory page is opened - url changed to https://www.saucedemo.com/inventory.html
 2. Opened within 2 secs</t>
+  </si>
+  <si>
+    <t>Test:</t>
   </si>
 </sst>
 </file>
@@ -573,28 +573,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,29 +892,29 @@
     <col min="4" max="4" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="6"/>
     </row>
@@ -922,7 +922,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="6"/>
     </row>
@@ -930,21 +930,21 @@
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
       <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
-        <v>2</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="6"/>
     </row>
@@ -952,7 +952,7 @@
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="6"/>
     </row>
@@ -960,21 +960,21 @@
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
       <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>3</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
-        <v>3</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>12</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -982,7 +982,7 @@
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -990,21 +990,21 @@
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
       <c r="C10" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
+      <c r="C11" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="D11" s="6"/>
     </row>
@@ -1012,7 +1012,7 @@
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="6"/>
     </row>
@@ -1020,21 +1020,21 @@
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>5</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
-        <v>5</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="6"/>
     </row>
@@ -1042,7 +1042,7 @@
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="6"/>
     </row>
@@ -1050,21 +1050,21 @@
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
       <c r="C16" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>6</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
-        <v>6</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>21</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="6"/>
     </row>
@@ -1072,7 +1072,7 @@
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
       <c r="C18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="6"/>
     </row>
@@ -1080,10 +1080,10 @@
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
       <c r="C19" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1178,18 +1178,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://www.saucedemo.com/" xr:uid="{F2CC4EAF-F6FB-4CBC-A3D3-61279BB69535}"/>

</xml_diff>

<commit_message>
added tests 3-7, new test cases
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Automation first steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D69F77-984E-4CDF-86C3-91CE66257485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8390CE-F05E-4713-B1F0-F1CC286DB650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Log in" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,18 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
-  <si>
-    <t>Goal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Steps</t>
   </si>
   <si>
     <t>Asserts</t>
-  </si>
-  <si>
-    <t>To check that user can log in with standard user.</t>
   </si>
   <si>
     <t>1. Open https://www.saucedemo.com/</t>
@@ -99,9 +94,6 @@
     </r>
   </si>
   <si>
-    <t>To check that error is displayed when username and password fields are empty</t>
-  </si>
-  <si>
     <t>2. Leave username empty
 Leave password field empty</t>
   </si>
@@ -123,9 +115,6 @@
   </si>
   <si>
     <t>1. Error is displayed with text "Epic sadface: Username is required"</t>
-  </si>
-  <si>
-    <t>To check that error is displayed when username field is empty</t>
   </si>
   <si>
     <r>
@@ -149,9 +138,6 @@
     <t>Error is displayed "Epic sadface: Username is required"</t>
   </si>
   <si>
-    <t>To check that error is displayed when pass is empty</t>
-  </si>
-  <si>
     <t>2. Input to username: 
 12345
 Leave password field empty</t>
@@ -160,7 +146,21 @@
     <t>Error is displayed "Epic sadface: Password is required"</t>
   </si>
   <si>
-    <t>To check that error is displayed when username does not exist</t>
+    <t>Error is displayed "Epic sadface: Username and password do not match any user in this service"</t>
+  </si>
+  <si>
+    <t>1. Inventory page is opened - url changed to https://www.saucedemo.com/inventory.html
+2. Opened within 2 secs</t>
+  </si>
+  <si>
+    <t>Test:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory page is opened - url changed to https://www.saucedemo.com/inventory.html
+</t>
+  </si>
+  <si>
+    <t>Url is not changed</t>
   </si>
   <si>
     <r>
@@ -177,7 +177,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">12345
+      <t xml:space="preserve">non-existent username
 </t>
     </r>
     <r>
@@ -202,12 +202,6 @@
       </rPr>
       <t>secret_sauce</t>
     </r>
-  </si>
-  <si>
-    <t>Error is displayed "Epic sadface: Username and password do not match any user in this service"</t>
-  </si>
-  <si>
-    <t>To check that error is displayed when pass does not match usename</t>
   </si>
   <si>
     <r>
@@ -247,15 +241,212 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>test</t>
-    </r>
-  </si>
-  <si>
-    <t>1. Inventory page is opened - url changed to https://www.saucedemo.com/inventory.html
-2. Opened within 2 secs</t>
-  </si>
-  <si>
-    <t>Test:</t>
+      <t>non-existent pass</t>
+    </r>
+  </si>
+  <si>
+    <t>Goal is to check that:</t>
+  </si>
+  <si>
+    <t>user can log in with standard user.</t>
+  </si>
+  <si>
+    <t>error is displayed when username and password fields are empty</t>
+  </si>
+  <si>
+    <t>error is displayed when username field is empty</t>
+  </si>
+  <si>
+    <t>error is displayed when pass is empty</t>
+  </si>
+  <si>
+    <t>error is displayed when username does not exist</t>
+  </si>
+  <si>
+    <t>error is displayed when pass does not match usename</t>
+  </si>
+  <si>
+    <t>username field is case sensitive</t>
+  </si>
+  <si>
+    <t>Password field is case sensitive</t>
+  </si>
+  <si>
+    <t>user can log in after 3 fail login attempts</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7. Click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9. Click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Input to 
+username: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>standard_user1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+password: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>secret_sauce</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.username: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>standard_user2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+same password</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6.username: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>standard_user3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+same password</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8. Input 
+Username: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>standard_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+same password</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -308,7 +499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -534,6 +725,32 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -541,11 +758,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -567,12 +781,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -596,6 +804,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -878,306 +1110,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" style="18" customWidth="1"/>
     <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="3" width="71.140625" customWidth="1"/>
     <col min="4" max="4" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
-        <v>1</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="4" t="s">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
         <v>5</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="7" t="s">
+      <c r="B14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="D16" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
-        <v>3</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
-        <v>4</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
-        <v>5</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
-        <v>6</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="6"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="22"/>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="6"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="22"/>
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="22"/>
+      <c r="C26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="6"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="6"/>
+      <c r="A29" s="17">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="6"/>
+      <c r="A32" s="17">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="17"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="A20:A28"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A5:A7"/>
@@ -1198,8 +1488,21 @@
     <hyperlink ref="C11" r:id="rId4" display="https://www.saucedemo.com/" xr:uid="{7FAE4C17-A388-4CBA-870A-C2CFC0324170}"/>
     <hyperlink ref="C14" r:id="rId5" display="https://www.saucedemo.com/" xr:uid="{4F164DC4-D8C6-463E-A163-F1C696B990C0}"/>
     <hyperlink ref="C17" r:id="rId6" display="https://www.saucedemo.com/" xr:uid="{BEC7E79B-6D83-4B35-81F0-A3B089F2FDD8}"/>
+    <hyperlink ref="C20" r:id="rId7" display="https://www.saucedemo.com/" xr:uid="{292FBD41-28C6-4214-8F09-02AD65AF9440}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B2B3A2-C83E-447E-84CC-0452A4A8720F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test case to reflect 1.1
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Automation first steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284B9896-2554-44A5-B550-9CB9B744B967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59A2F2D-5D37-416A-A4D2-ACF8B65C7457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Steps</t>
   </si>
@@ -531,6 +531,55 @@
   </si>
   <si>
     <t>Page opens within 2 secs.</t>
+  </si>
+  <si>
+    <t>user can log in with standard_user, problem_user, performance_glitch_user, error_user, visual_user</t>
+  </si>
+  <si>
+    <t>3. Click Login</t>
+  </si>
+  <si>
+    <t>Inventory page is opened - url changed to https://www.saucedemo.com/inventory.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Run same test with each username:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>standard_user, problem_user, performance_glitch_user, error_user, visual_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+and password:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>secret_sauce</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -631,55 +680,55 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -961,11 +1010,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,452 +1026,491 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="6" t="s">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>2</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>3</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>4</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>5</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>6</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
+        <v>7</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="39" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
+        <v>8</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
+        <v>9</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6" t="s">
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="D46" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
+        <v>10</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>5</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>6</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>7</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>8</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>9</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="16">
-        <v>10</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="6" t="s">
+      <c r="D48" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
+    <row r="49" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="15"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="A26:A34"/>
+  <mergeCells count="20">
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A30:A38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://www.saucedemo.com/" xr:uid="{F2CC4EAF-F6FB-4CBC-A3D3-61279BB69535}"/>
-    <hyperlink ref="C6" r:id="rId2" display="https://www.saucedemo.com/" xr:uid="{1E4E3F2E-370A-4AFA-812B-A0FF20D1F188}"/>
-    <hyperlink ref="C10" r:id="rId3" display="https://www.saucedemo.com/" xr:uid="{81EF4364-6C27-4550-9C2D-8827CB9E8EB0}"/>
-    <hyperlink ref="C14" r:id="rId4" display="https://www.saucedemo.com/" xr:uid="{7FAE4C17-A388-4CBA-870A-C2CFC0324170}"/>
-    <hyperlink ref="C18" r:id="rId5" display="https://www.saucedemo.com/" xr:uid="{4F164DC4-D8C6-463E-A163-F1C696B990C0}"/>
-    <hyperlink ref="C22" r:id="rId6" display="https://www.saucedemo.com/" xr:uid="{BEC7E79B-6D83-4B35-81F0-A3B089F2FDD8}"/>
-    <hyperlink ref="C26" r:id="rId7" display="https://www.saucedemo.com/" xr:uid="{292FBD41-28C6-4214-8F09-02AD65AF9440}"/>
-    <hyperlink ref="C36" r:id="rId8" display="https://www.saucedemo.com/" xr:uid="{02E80879-6131-42E9-9CEB-97FC2B5A49D6}"/>
-    <hyperlink ref="C40" r:id="rId9" display="https://www.saucedemo.com/" xr:uid="{F73CD8F2-E31B-48C1-B463-B0C4566E975C}"/>
-    <hyperlink ref="C44" r:id="rId10" display="https://www.saucedemo.com/" xr:uid="{A85D5AB7-9147-4807-B216-D988626D5D5E}"/>
+    <hyperlink ref="C14" r:id="rId2" display="https://www.saucedemo.com/" xr:uid="{81EF4364-6C27-4550-9C2D-8827CB9E8EB0}"/>
+    <hyperlink ref="C18" r:id="rId3" display="https://www.saucedemo.com/" xr:uid="{7FAE4C17-A388-4CBA-870A-C2CFC0324170}"/>
+    <hyperlink ref="C22" r:id="rId4" display="https://www.saucedemo.com/" xr:uid="{4F164DC4-D8C6-463E-A163-F1C696B990C0}"/>
+    <hyperlink ref="C26" r:id="rId5" display="https://www.saucedemo.com/" xr:uid="{BEC7E79B-6D83-4B35-81F0-A3B089F2FDD8}"/>
+    <hyperlink ref="C30" r:id="rId6" display="https://www.saucedemo.com/" xr:uid="{292FBD41-28C6-4214-8F09-02AD65AF9440}"/>
+    <hyperlink ref="C40" r:id="rId7" display="https://www.saucedemo.com/" xr:uid="{02E80879-6131-42E9-9CEB-97FC2B5A49D6}"/>
+    <hyperlink ref="C44" r:id="rId8" display="https://www.saucedemo.com/" xr:uid="{F73CD8F2-E31B-48C1-B463-B0C4566E975C}"/>
+    <hyperlink ref="C48" r:id="rId9" display="https://www.saucedemo.com/" xr:uid="{A85D5AB7-9147-4807-B216-D988626D5D5E}"/>
+    <hyperlink ref="C6" r:id="rId10" display="https://www.saucedemo.com/" xr:uid="{D4D2FB36-F64B-46A3-ABE1-D335CA1DB204}"/>
+    <hyperlink ref="C10" r:id="rId11" display="https://www.saucedemo.com/" xr:uid="{1E4E3F2E-370A-4AFA-812B-A0FF20D1F188}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
structured tests: added suits, list of tests
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Automation first steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59A2F2D-5D37-416A-A4D2-ACF8B65C7457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C023C7-D0BB-4D9B-BAD6-C79CCE91D2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log in" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
+    <sheet name="Inventory" sheetId="2" r:id="rId2"/>
+    <sheet name="Side Nav" sheetId="5" r:id="rId3"/>
+    <sheet name="Single item page" sheetId="4" r:id="rId4"/>
+    <sheet name="Checkout" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,13 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
-  <si>
-    <t>Steps</t>
-  </si>
-  <si>
-    <t>Asserts</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="94">
   <si>
     <t>1. Open https://www.saucedemo.com/</t>
   </si>
@@ -579,6 +576,1382 @@
         <charset val="204"/>
       </rPr>
       <t>secret_sauce</t>
+    </r>
+  </si>
+  <si>
+    <t>Steps:</t>
+  </si>
+  <si>
+    <t>Asserts:</t>
+  </si>
+  <si>
+    <t>Elements are presented on the page</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.saucedemo.com/</t>
+  </si>
+  <si>
+    <t>Side nav is opened. 
+It contains:
+All Items,
+About
+Logout
+Reset App State</t>
+  </si>
+  <si>
+    <t>Cart page is opened</t>
+  </si>
+  <si>
+    <t>side nav is opened</t>
+  </si>
+  <si>
+    <t>Expected(only essentials):</t>
+  </si>
+  <si>
+    <t>side nav is not displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elements are presented on the page:
+Header 'Swag Labs'
+Invetory list with inventory items
+shopping cart icon
+burger menu icon
+social icons
+Add to cart button for each list item 
+Price for each list item
+sorting element
+footer copy text </t>
+  </si>
+  <si>
+    <t>Preconditions</t>
+  </si>
+  <si>
+    <t>1. Wait till inventory page is opened.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Input
+username: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>standard_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+pass: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secret_sauce</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Clicking</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burger menu icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> inventory page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Input
+username: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">standard_user </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+pass: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secret_sauce</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>burger menu icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Side nav</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> can be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>closed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with close button on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Click burger menu icon</t>
+  </si>
+  <si>
+    <t>2. Click Close button</t>
+  </si>
+  <si>
+    <t>1. Click Cart icon</t>
+  </si>
+  <si>
+    <t>2. Click burger menu icon</t>
+  </si>
+  <si>
+    <t>3. Click Close button</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens cart page</t>
+    </r>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Side nav</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> can be</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> closed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with close button on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <t>Adding to cart</t>
+  </si>
+  <si>
+    <t>removing from cart</t>
+  </si>
+  <si>
+    <t>back to products link</t>
+  </si>
+  <si>
+    <r>
+      <t>Clicking</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burger menu icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> single item page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Side nav</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> can be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>closed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with close button on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>single item page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to inventory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>About</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to about page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page logs out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reset app state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page resets app state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to inventory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>About</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to about page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page logs out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reset app state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page resets app state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to inventory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>About</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to about page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reset app state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page resets app state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Single item </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page logs out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking each item's </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens a new page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking each item's </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>header</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens a new page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Add to cart </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>adds an item to cart</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> removes the item from cart</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>twitter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon open twitter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>facebook</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cion open facebook </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Linkedin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon opens linkedin</t>
+    </r>
+  </si>
+  <si>
+    <t>default sorting in alphabetical asc</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">user can sort items in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desc alphbtical</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> order</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">user can sort by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>price from low to high</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">user can sort by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>price from high to low</t>
     </r>
   </si>
 </sst>
@@ -586,7 +1959,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,6 +1998,82 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -646,7 +2095,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -669,12 +2118,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -724,10 +2241,124 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1012,9 +2643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,46 +2658,46 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="28">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
-        <v>1</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1079,30 +2710,30 @@
       <c r="A6" s="17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>39</v>
+      <c r="B6" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
-      <c r="B7" s="19"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
-      <c r="B8" s="19"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1115,30 +2746,30 @@
       <c r="A10" s="17">
         <v>2</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>19</v>
+      <c r="B10" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
-      <c r="B11" s="19"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
-      <c r="B12" s="19"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1151,30 +2782,30 @@
       <c r="A14" s="17">
         <v>3</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>20</v>
+      <c r="B14" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
-      <c r="B15" s="19"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
-      <c r="B16" s="19"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1187,30 +2818,30 @@
       <c r="A18" s="17">
         <v>4</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>21</v>
+      <c r="B18" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
-      <c r="B19" s="19"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
-      <c r="B20" s="19"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1223,30 +2854,30 @@
       <c r="A22" s="17">
         <v>5</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>22</v>
+      <c r="B22" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
-      <c r="B23" s="19"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
-      <c r="B24" s="19"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1259,30 +2890,30 @@
       <c r="A26" s="17">
         <v>6</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>23</v>
+      <c r="B26" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
-      <c r="B27" s="19"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
-      <c r="B28" s="19"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1295,84 +2926,84 @@
       <c r="A30" s="17">
         <v>7</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>25</v>
+      <c r="B30" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
-      <c r="B31" s="18"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
-      <c r="B32" s="18"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
-      <c r="B33" s="18"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
-      <c r="B34" s="18"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
-      <c r="B35" s="18"/>
+      <c r="B35" s="19"/>
       <c r="C35" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
-      <c r="B36" s="18"/>
+      <c r="B36" s="19"/>
       <c r="C36" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
-      <c r="B37" s="18"/>
+      <c r="B37" s="19"/>
       <c r="C37" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
-      <c r="B38" s="18"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1385,30 +3016,30 @@
       <c r="A40" s="17">
         <v>8</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>35</v>
+      <c r="B40" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
-      <c r="B42" s="18"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1421,30 +3052,30 @@
       <c r="A44" s="17">
         <v>9</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>24</v>
+      <c r="B44" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
-      <c r="B45" s="18"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
-      <c r="B46" s="18"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1458,13 +3089,13 @@
         <v>10</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1475,12 +3106,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A30:A38"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A10:A12"/>
@@ -1489,12 +3120,12 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://www.saucedemo.com/" xr:uid="{F2CC4EAF-F6FB-4CBC-A3D3-61279BB69535}"/>
@@ -1516,12 +3147,1362 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B2B3A2-C83E-447E-84CC-0452A4A8720F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
+        <v>1</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>2</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <v>3</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="36"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+    </row>
+    <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>4</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="35"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="35"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="35"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="34">
+        <v>5</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="40">
+        <v>6</v>
+      </c>
+      <c r="B22" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="47">
+        <v>7</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="37"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+    </row>
+    <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="47">
+        <v>8</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="37"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+    </row>
+    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="47">
+        <v>9</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="37"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="47">
+        <v>10</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+    </row>
+    <row r="34" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="57">
+        <v>11</v>
+      </c>
+      <c r="B34" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="37"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+    </row>
+    <row r="36" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="47">
+        <v>12</v>
+      </c>
+      <c r="B36" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="37"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+    </row>
+    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="47">
+        <v>13</v>
+      </c>
+      <c r="B38" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="37"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="44"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="44"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="44"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="44"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="44"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="44"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="44"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="44"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="44"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="44"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="44"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="44"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="44"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="44"/>
+      <c r="B53" s="54"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="44"/>
+      <c r="B54" s="54"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="44"/>
+      <c r="B55" s="54"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="44"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="36"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="44"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="44"/>
+      <c r="B58" s="54"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="36"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="44"/>
+      <c r="B59" s="54"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="44"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="44"/>
+      <c r="B61" s="54"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="36"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="44"/>
+      <c r="B62" s="54"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="44"/>
+      <c r="B63" s="54"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="44"/>
+      <c r="B64" s="54"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="44"/>
+      <c r="B65" s="54"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="45"/>
+      <c r="B66" s="55"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="43"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="45"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="45"/>
+      <c r="B68" s="55"/>
+      <c r="C68" s="43"/>
+      <c r="D68" s="43"/>
+      <c r="E68" s="43"/>
+      <c r="F68" s="43"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="45"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="43"/>
+      <c r="F69" s="43"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="45"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CB27FF-4E4D-406E-80C2-3529D9AEA90A}">
+  <dimension ref="A1:F48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="48">
+        <v>1</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="35"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="48">
+        <v>2</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="48">
+        <v>3</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="35"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="35"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+    </row>
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="48">
+        <v>4</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="36"/>
+    </row>
+    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="36"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="46">
+        <v>5</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="46"/>
+      <c r="B19" s="35"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="46"/>
+      <c r="B20" s="35"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="46">
+        <v>6</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="46"/>
+      <c r="B23" s="35"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="46"/>
+      <c r="B24" s="35"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="A10:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8168AB64-C060-49DD-9E77-E077B140F3A3}">
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
+        <v>1</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+    </row>
+    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B7EFAF-D28D-4990-84F2-67255EDBCD5F}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" customWidth="1"/>
+    <col min="6" max="6" width="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
+        <v>1</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 4 login page test cases
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Automation first steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C023C7-D0BB-4D9B-BAD6-C79CCE91D2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413F64AD-1DC0-4C15-9509-538258C03D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log in" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="106">
   <si>
     <t>1. Open https://www.saucedemo.com/</t>
   </si>
@@ -1953,6 +1953,46 @@
       </rPr>
       <t>price from high to low</t>
     </r>
+  </si>
+  <si>
+    <t>Error is displayed when trying to reach /inventory while not logged in</t>
+  </si>
+  <si>
+    <t>Error is displayed : 
+'Epic sadface: You can only access '/inventory.html' when you are logged in.'</t>
+  </si>
+  <si>
+    <t>Error is displayed when trying to reach /cart while not logged in</t>
+  </si>
+  <si>
+    <t>Error is displayed when trying to reach /checkout-step-one while not logged in</t>
+  </si>
+  <si>
+    <t>Error is displayed when trying to reach /inventory-item while not logged in</t>
+  </si>
+  <si>
+    <t>Error is displayed : 
+'Epic sadface: You can only access '/cart.html' when you are logged in.'</t>
+  </si>
+  <si>
+    <t>Error is displayed : 
+'Epic sadface: You can only access '/checkout-step-one.html' when you are logged in'</t>
+  </si>
+  <si>
+    <t>Error is displayed : 
+'Epic sadface: You can only access '/inventory-item.html' when you are logged in.'</t>
+  </si>
+  <si>
+    <t>1. Open https://www.saucedemo.com/cart.html</t>
+  </si>
+  <si>
+    <t>1. Open https://www.saucedemo.com/inventory-item.html?id=4</t>
+  </si>
+  <si>
+    <t>1. Open https://www.saucedemo.com/checkout-step-one.html</t>
+  </si>
+  <si>
+    <t>1. Open https://www.saucedemo.com/inventory.html</t>
   </si>
 </sst>
 </file>
@@ -2191,15 +2231,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2233,41 +2270,76 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2288,24 +2360,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2315,21 +2381,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2342,23 +2393,26 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2641,477 +2695,608 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
-    <col min="3" max="3" width="71.140625" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" customWidth="1"/>
+    <col min="1" max="1" width="11" style="35" customWidth="1"/>
+    <col min="2" max="2" width="56" style="14" customWidth="1"/>
+    <col min="3" max="3" width="71.140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="4" t="s">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="39"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="4" t="s">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="55"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="4" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="36"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="4" t="s">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="36"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="55"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
         <v>2</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="4" t="s">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="36"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="4" t="s">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="55"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="36">
         <v>3</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="4" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="4" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="55"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="36">
         <v>4</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="4" t="s">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="4" t="s">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="55"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="36">
         <v>5</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="4" t="s">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="4" t="s">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="55"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="36">
         <v>6</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="4" t="s">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="4" t="s">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+    <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="55"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="36">
         <v>7</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="4" t="s">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="36"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="4" t="s">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="4" t="s">
+    <row r="33" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="4" t="s">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="4" t="s">
+    <row r="35" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="4" t="s">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="36"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="4" t="s">
+    <row r="37" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="10" t="s">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="36"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="9"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
+    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="55"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="36">
         <v>8</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="10" t="s">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="10" t="s">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="9"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+    <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="55"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="36">
         <v>9</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="10" t="s">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="36"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="10" t="s">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="13">
+    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="55"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
         <v>10</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
+    <row r="49" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="56"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="55"/>
+    </row>
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="58">
+        <v>11</v>
+      </c>
+      <c r="B50" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="56"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="55"/>
+    </row>
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="58">
+        <v>13</v>
+      </c>
+      <c r="B52" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" s="59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="56"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="55"/>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="58">
+        <v>14</v>
+      </c>
+      <c r="B54" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="56"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="55"/>
+    </row>
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="58">
+        <v>15</v>
+      </c>
+      <c r="B56" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D56" s="59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="56"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="55"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="58"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+    </row>
+    <row r="59" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="56"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="55"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="58"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+    </row>
+    <row r="61" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="56"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="55"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="60"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="60"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A10:A12"/>
@@ -3120,28 +3305,15 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A30:A38"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://www.saucedemo.com/" xr:uid="{F2CC4EAF-F6FB-4CBC-A3D3-61279BB69535}"/>
-    <hyperlink ref="C14" r:id="rId2" display="https://www.saucedemo.com/" xr:uid="{81EF4364-6C27-4550-9C2D-8827CB9E8EB0}"/>
-    <hyperlink ref="C18" r:id="rId3" display="https://www.saucedemo.com/" xr:uid="{7FAE4C17-A388-4CBA-870A-C2CFC0324170}"/>
-    <hyperlink ref="C22" r:id="rId4" display="https://www.saucedemo.com/" xr:uid="{4F164DC4-D8C6-463E-A163-F1C696B990C0}"/>
-    <hyperlink ref="C26" r:id="rId5" display="https://www.saucedemo.com/" xr:uid="{BEC7E79B-6D83-4B35-81F0-A3B089F2FDD8}"/>
-    <hyperlink ref="C30" r:id="rId6" display="https://www.saucedemo.com/" xr:uid="{292FBD41-28C6-4214-8F09-02AD65AF9440}"/>
-    <hyperlink ref="C40" r:id="rId7" display="https://www.saucedemo.com/" xr:uid="{02E80879-6131-42E9-9CEB-97FC2B5A49D6}"/>
-    <hyperlink ref="C44" r:id="rId8" display="https://www.saucedemo.com/" xr:uid="{F73CD8F2-E31B-48C1-B463-B0C4566E975C}"/>
-    <hyperlink ref="C48" r:id="rId9" display="https://www.saucedemo.com/" xr:uid="{A85D5AB7-9147-4807-B216-D988626D5D5E}"/>
-    <hyperlink ref="C6" r:id="rId10" display="https://www.saucedemo.com/" xr:uid="{D4D2FB36-F64B-46A3-ABE1-D335CA1DB204}"/>
-    <hyperlink ref="C10" r:id="rId11" display="https://www.saucedemo.com/" xr:uid="{1E4E3F2E-370A-4AFA-812B-A0FF20D1F188}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3149,663 +3321,671 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B2B3A2-C83E-447E-84CC-0452A4A8720F}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="22" customWidth="1"/>
-    <col min="3" max="3" width="55.85546875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="52.5703125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="34">
+      <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="45"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="36" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
+      <c r="A6" s="45">
         <v>2</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="36" t="s">
+      <c r="A7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="36" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="34">
+      <c r="A10" s="45">
         <v>3</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="36"/>
+      <c r="C10" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="22">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="36"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
+      <c r="A14" s="45">
         <v>4</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="35"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="47"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="35"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="47"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="35"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="47"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="34">
+      <c r="A18" s="45">
         <v>5</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+      <c r="A19" s="45"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="A20" s="45"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="40">
+      <c r="A22" s="48">
         <v>6</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="47">
+      <c r="A26" s="30">
         <v>7</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
     </row>
     <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="47">
+      <c r="A28" s="30">
         <v>8</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
     </row>
     <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="47">
+      <c r="A30" s="30">
         <v>9</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="47">
+      <c r="A32" s="30">
         <v>10</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
     </row>
     <row r="34" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="57">
+      <c r="A34" s="35">
         <v>11</v>
       </c>
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="47">
+      <c r="A36" s="30">
         <v>12</v>
       </c>
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="47">
+      <c r="A38" s="30">
         <v>13</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
+      <c r="A41" s="27"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-      <c r="B44" s="54"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="54"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="54"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
-      <c r="B49" s="54"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="54"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
-      <c r="B51" s="54"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
-      <c r="B52" s="54"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
-      <c r="B53" s="54"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="54"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="54"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
+      <c r="A56" s="27"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
-      <c r="B57" s="54"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
-      <c r="B58" s="54"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
-      <c r="B59" s="54"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
-      <c r="B60" s="54"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
-      <c r="B61" s="54"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
-      <c r="B62" s="54"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
-      <c r="B63" s="54"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="54"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
+      <c r="A64" s="27"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="44"/>
-      <c r="B65" s="54"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
+      <c r="A65" s="27"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="45"/>
-      <c r="B66" s="55"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
+      <c r="A66" s="28"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="45"/>
-      <c r="B67" s="55"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
+      <c r="A67" s="28"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="45"/>
-      <c r="B68" s="55"/>
-      <c r="C68" s="43"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="45"/>
-      <c r="B69" s="55"/>
-      <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="45"/>
-      <c r="B70" s="55"/>
-      <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
+      <c r="A70" s="28"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3823,344 +4003,339 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48">
+      <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="47" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="52"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="35"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="48">
+      <c r="A6" s="51">
         <v>2</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="36" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="22" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36" t="s">
+      <c r="A8" s="52"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="36"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="48">
+      <c r="A10" s="51">
         <v>3</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="35" t="s">
+      <c r="E10" s="22"/>
+      <c r="F10" s="47" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36" t="s">
+      <c r="A11" s="52"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="35"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36" t="s">
+      <c r="A12" s="52"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="35"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="48">
+      <c r="A14" s="51">
         <v>4</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="36"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36" t="s">
+      <c r="A15" s="52"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="36"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36" t="s">
+      <c r="A16" s="52"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36" t="s">
+      <c r="E16" s="22"/>
+      <c r="F16" s="22" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="46">
+      <c r="A18" s="29">
         <v>5</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="47" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="47"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="47"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="46">
+      <c r="A22" s="29">
         <v>6</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="47" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="47"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="35"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="47"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="14" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="14" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="14" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A2:A4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B6:B8"/>
@@ -4168,6 +4343,11 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4193,66 +4373,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34">
+      <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="45"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -4293,12 +4473,12 @@
       <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -4445,58 +4625,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="34">
+      <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added tests 11-14. errors on reaching endpoints while not logged in
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Automation first steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413F64AD-1DC0-4C15-9509-538258C03D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A4B089-5BB0-4826-9879-4C81F925A418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2336,11 +2336,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2361,15 +2382,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2381,6 +2402,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2389,30 +2413,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2699,7 +2699,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,10 +2726,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="38">
+      <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="48" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -2738,16 +2738,16 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="42"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2760,10 +2760,10 @@
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="55"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="36">
+      <c r="A6" s="43">
         <v>1.1000000000000001</v>
       </c>
       <c r="B6" s="44" t="s">
@@ -2775,7 +2775,7 @@
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="44"/>
       <c r="C7" s="3" t="s">
         <v>40</v>
@@ -2783,7 +2783,7 @@
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="44"/>
       <c r="C8" s="3" t="s">
         <v>38</v>
@@ -2797,10 +2797,10 @@
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="55"/>
+      <c r="E9" s="36"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
+      <c r="A10" s="43">
         <v>2</v>
       </c>
       <c r="B10" s="44" t="s">
@@ -2812,7 +2812,7 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="44"/>
       <c r="C11" s="3" t="s">
         <v>3</v>
@@ -2820,7 +2820,7 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="44"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
@@ -2834,10 +2834,10 @@
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="55"/>
+      <c r="E13" s="36"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="36">
+      <c r="A14" s="43">
         <v>3</v>
       </c>
       <c r="B14" s="44" t="s">
@@ -2849,7 +2849,7 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="44"/>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -2857,7 +2857,7 @@
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="44"/>
       <c r="C16" s="3" t="s">
         <v>4</v>
@@ -2871,10 +2871,10 @@
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="55"/>
+      <c r="E17" s="36"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="36">
+      <c r="A18" s="43">
         <v>4</v>
       </c>
       <c r="B18" s="44" t="s">
@@ -2886,7 +2886,7 @@
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="44"/>
       <c r="C19" s="3" t="s">
         <v>7</v>
@@ -2894,7 +2894,7 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="44"/>
       <c r="C20" s="3" t="s">
         <v>4</v>
@@ -2908,10 +2908,10 @@
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="55"/>
+      <c r="E21" s="36"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="36">
+      <c r="A22" s="43">
         <v>5</v>
       </c>
       <c r="B22" s="44" t="s">
@@ -2923,7 +2923,7 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="44"/>
       <c r="C23" s="3" t="s">
         <v>13</v>
@@ -2931,7 +2931,7 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="44"/>
       <c r="C24" s="3" t="s">
         <v>4</v>
@@ -2945,10 +2945,10 @@
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="55"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="36">
+      <c r="A26" s="43">
         <v>6</v>
       </c>
       <c r="B26" s="44" t="s">
@@ -2960,7 +2960,7 @@
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="44"/>
       <c r="C27" s="3" t="s">
         <v>14</v>
@@ -2968,7 +2968,7 @@
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="44"/>
       <c r="C28" s="3" t="s">
         <v>4</v>
@@ -2982,13 +2982,13 @@
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="55"/>
+      <c r="E29" s="36"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="36">
+      <c r="A30" s="43">
         <v>7</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="51" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="14" t="s">
@@ -2997,16 +2997,16 @@
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="37"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="37"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="3" t="s">
         <v>4</v>
       </c>
@@ -3015,16 +3015,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="37"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="B34" s="37"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="3" t="s">
         <v>24</v>
       </c>
@@ -3033,16 +3033,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
-      <c r="B36" s="37"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="3" t="s">
         <v>25</v>
       </c>
@@ -3051,16 +3051,16 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
-      <c r="B37" s="37"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="37"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="9" t="s">
         <v>26</v>
       </c>
@@ -3073,13 +3073,13 @@
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="55"/>
+      <c r="E39" s="36"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="36">
+      <c r="A40" s="43">
         <v>8</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="51" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="14" t="s">
@@ -3088,16 +3088,16 @@
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
-      <c r="B41" s="37"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
-      <c r="B42" s="37"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="9" t="s">
         <v>4</v>
       </c>
@@ -3110,13 +3110,13 @@
       <c r="B43" s="8"/>
       <c r="C43" s="11"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="55"/>
+      <c r="E43" s="36"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="36">
+      <c r="A44" s="43">
         <v>9</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="51" t="s">
         <v>22</v>
       </c>
       <c r="C44" s="14" t="s">
@@ -3125,16 +3125,16 @@
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
-      <c r="B45" s="37"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
-      <c r="B46" s="37"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="9" t="s">
         <v>4</v>
       </c>
@@ -3147,7 +3147,7 @@
       <c r="B47" s="8"/>
       <c r="C47" s="11"/>
       <c r="D47" s="8"/>
-      <c r="E47" s="55"/>
+      <c r="E47" s="36"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
@@ -3164,139 +3164,139 @@
       </c>
     </row>
     <row r="49" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="56"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="55"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="36"/>
     </row>
     <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="58">
+      <c r="A50" s="39">
         <v>11</v>
       </c>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="40" t="s">
         <v>94</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D50" s="59" t="s">
+      <c r="D50" s="40" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="55"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="36"/>
     </row>
     <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="58">
-        <v>13</v>
-      </c>
-      <c r="B52" s="59" t="s">
+      <c r="A52" s="39">
+        <v>12</v>
+      </c>
+      <c r="B52" s="40" t="s">
         <v>96</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D52" s="59" t="s">
+      <c r="D52" s="40" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="55"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="36"/>
     </row>
     <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="58">
-        <v>14</v>
-      </c>
-      <c r="B54" s="59" t="s">
+      <c r="A54" s="39">
+        <v>13</v>
+      </c>
+      <c r="B54" s="40" t="s">
         <v>97</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="D54" s="59" t="s">
+      <c r="D54" s="40" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="56"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="61"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="55"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="58">
-        <v>15</v>
-      </c>
-      <c r="B56" s="59" t="s">
+      <c r="A56" s="39">
+        <v>14</v>
+      </c>
+      <c r="B56" s="40" t="s">
         <v>98</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D56" s="59" t="s">
+      <c r="D56" s="40" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="55"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="36"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="58"/>
-      <c r="B58" s="59"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
     </row>
     <row r="59" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="56"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="57"/>
-      <c r="E59" s="55"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="36"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="58"/>
-      <c r="B60" s="59"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="59"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
     </row>
     <row r="61" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="56"/>
-      <c r="B61" s="57"/>
-      <c r="C61" s="57"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="55"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="36"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="60"/>
+      <c r="B69" s="41"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="60"/>
+      <c r="B72" s="41"/>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="60"/>
+      <c r="B75" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A30:A38"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A10:A12"/>
@@ -3305,12 +3305,12 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3357,10 +3357,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="45">
+      <c r="A2" s="53">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="52" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -3375,8 +3375,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
@@ -3385,8 +3385,8 @@
       <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
@@ -3403,10 +3403,10 @@
       <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45">
+      <c r="A6" s="53">
         <v>2</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="52" t="s">
         <v>63</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -3421,8 +3421,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="22" t="s">
         <v>55</v>
       </c>
@@ -3431,8 +3431,8 @@
       <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="46"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
@@ -3449,10 +3449,10 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="45">
+      <c r="A10" s="53">
         <v>3</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="52" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -3464,8 +3464,8 @@
       <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="46"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="22" t="s">
         <v>55</v>
       </c>
@@ -3474,8 +3474,8 @@
       <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="46"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="22" t="s">
         <v>38</v>
       </c>
@@ -3492,32 +3492,32 @@
       <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45">
+      <c r="A14" s="53">
         <v>4</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="52" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
-      <c r="F14" s="47"/>
+      <c r="F14" s="54"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="46"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="22"/>
       <c r="D15" s="18"/>
       <c r="E15" s="22"/>
-      <c r="F15" s="47"/>
+      <c r="F15" s="54"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="46"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="22"/>
       <c r="D16" s="18"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="47"/>
+      <c r="F16" s="54"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
@@ -3528,7 +3528,7 @@
       <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="45">
+      <c r="A18" s="53">
         <v>5</v>
       </c>
       <c r="B18" s="16" t="s">
@@ -3536,10 +3536,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="53"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="53"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
@@ -3550,10 +3550,10 @@
       <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="48">
+      <c r="A22" s="55">
         <v>6</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="52" t="s">
         <v>86</v>
       </c>
       <c r="C22" s="22"/>
@@ -3562,16 +3562,16 @@
       <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="46"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="46"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="22"/>
       <c r="D24" s="25"/>
       <c r="E24" s="22"/>
@@ -3974,18 +3974,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="A22:A24"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="A22:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4031,10 +4031,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51">
+      <c r="A2" s="59">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="54" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -4044,29 +4044,29 @@
         <v>58</v>
       </c>
       <c r="E2" s="22"/>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="54" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="47"/>
+      <c r="F3" s="54"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="47"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="22"/>
-      <c r="F4" s="47"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
@@ -4077,10 +4077,10 @@
       <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="51">
+      <c r="A6" s="59">
         <v>2</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="58" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -4095,8 +4095,8 @@
       <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="47"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="22" t="s">
         <v>55</v>
       </c>
@@ -4109,8 +4109,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="47"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
@@ -4127,10 +4127,10 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="51">
+      <c r="A10" s="59">
         <v>3</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="54" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -4140,29 +4140,29 @@
         <v>58</v>
       </c>
       <c r="E10" s="22"/>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="54" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="22" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="47"/>
+      <c r="F11" s="54"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="22"/>
-      <c r="F12" s="47"/>
+      <c r="F12" s="54"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -4173,10 +4173,10 @@
       <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="51">
+      <c r="A14" s="59">
         <v>4</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="54" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -4191,8 +4191,8 @@
       <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="22" t="s">
         <v>55</v>
       </c>
@@ -4205,8 +4205,8 @@
       <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="22" t="s">
         <v>38</v>
       </c>
@@ -4230,17 +4230,17 @@
       <c r="A18" s="29">
         <v>5</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="54" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="47"/>
+      <c r="B19" s="54"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
-      <c r="B20" s="47"/>
+      <c r="B20" s="54"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
@@ -4254,17 +4254,17 @@
       <c r="A22" s="29">
         <v>6</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="54" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="47"/>
+      <c r="B23" s="54"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
-      <c r="B24" s="47"/>
+      <c r="B24" s="54"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
@@ -4336,6 +4336,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A2:A4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B6:B8"/>
@@ -4343,11 +4348,6 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4393,10 +4393,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45">
+      <c r="A2" s="53">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="54" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -4407,8 +4407,8 @@
       <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
@@ -4417,8 +4417,8 @@
       <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="47"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
@@ -4645,26 +4645,26 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="45">
+      <c r="A2" s="53">
         <v>1</v>
       </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="54"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="47"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>

</xml_diff>

<commit_message>
Adde First Inventory page test checking that elements are displayed
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Automation first steps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A4B089-5BB0-4826-9879-4C81F925A418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE86777-78A5-44AF-BEA3-F8448B13B722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log in" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="105">
   <si>
     <t>1. Open https://www.saucedemo.com/</t>
   </si>
@@ -611,1388 +611,1384 @@
     <t>side nav is not displayed</t>
   </si>
   <si>
+    <t>Preconditions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Input
+username: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>standard_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+pass: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secret_sauce</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Clicking</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burger menu icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> inventory page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Input
+username: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">standard_user </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+pass: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secret_sauce</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>burger menu icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Side nav</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> can be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>closed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with close button on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Click burger menu icon</t>
+  </si>
+  <si>
+    <t>2. Click Close button</t>
+  </si>
+  <si>
+    <t>1. Click Cart icon</t>
+  </si>
+  <si>
+    <t>2. Click burger menu icon</t>
+  </si>
+  <si>
+    <t>3. Click Close button</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens cart page</t>
+    </r>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Side nav</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> can be</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> closed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with close button on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <t>Adding to cart</t>
+  </si>
+  <si>
+    <t>removing from cart</t>
+  </si>
+  <si>
+    <t>back to products link</t>
+  </si>
+  <si>
+    <r>
+      <t>Clicking</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burger menu icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> single item page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Side nav</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> can be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>closed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with close button on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>single item page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to inventory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>About</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to about page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page logs out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reset app state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page resets app state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to inventory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>About</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to about page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page logs out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reset app state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page resets app state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to inventory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>About</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page redirects to about page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reset app state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page resets app state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Single item </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page logs out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking each item's </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens a new page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking each item's </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>header</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens a new page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Add to cart </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>adds an item to cart</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> removes the item from cart</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>twitter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon open twitter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>facebook</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cion open facebook </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Linkedin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon opens linkedin</t>
+    </r>
+  </si>
+  <si>
+    <t>default sorting in alphabetical asc</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">user can sort items in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desc alphbtical</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> order</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">user can sort by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>price from low to high</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">user can sort by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>price from high to low</t>
+    </r>
+  </si>
+  <si>
+    <t>Error is displayed when trying to reach /inventory while not logged in</t>
+  </si>
+  <si>
+    <t>Error is displayed : 
+'Epic sadface: You can only access '/inventory.html' when you are logged in.'</t>
+  </si>
+  <si>
+    <t>Error is displayed when trying to reach /cart while not logged in</t>
+  </si>
+  <si>
+    <t>Error is displayed when trying to reach /checkout-step-one while not logged in</t>
+  </si>
+  <si>
+    <t>Error is displayed when trying to reach /inventory-item while not logged in</t>
+  </si>
+  <si>
+    <t>Error is displayed : 
+'Epic sadface: You can only access '/cart.html' when you are logged in.'</t>
+  </si>
+  <si>
+    <t>Error is displayed : 
+'Epic sadface: You can only access '/checkout-step-one.html' when you are logged in'</t>
+  </si>
+  <si>
+    <t>Error is displayed : 
+'Epic sadface: You can only access '/inventory-item.html' when you are logged in.'</t>
+  </si>
+  <si>
+    <t>1. Open https://www.saucedemo.com/cart.html</t>
+  </si>
+  <si>
+    <t>1. Open https://www.saucedemo.com/inventory-item.html?id=4</t>
+  </si>
+  <si>
+    <t>1. Open https://www.saucedemo.com/checkout-step-one.html</t>
+  </si>
+  <si>
+    <t>1. Open https://www.saucedemo.com/inventory.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elements are presented on the page:
 Header 'Swag Labs'
 Invetory list with inventory items
-shopping cart icon
-burger menu icon
+Price, image and Add to cart button for each item
+burger menu element
 social icons
-Add to cart button for each list item 
-Price for each list item
+shopping cart element
 sorting element
 footer copy text </t>
-  </si>
-  <si>
-    <t>Preconditions</t>
-  </si>
-  <si>
-    <t>1. Wait till inventory page is opened.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2. Input
-username: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>standard_user</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-pass: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>secret_sauce</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Clicking</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> burger menu icon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> on the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> inventory page</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2. Input
-username: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">standard_user </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-pass: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>secret_sauce</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>burger menu icon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cart</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>page</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Side nav</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> can be </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>closed</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> with close button on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cart</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page</t>
-    </r>
-  </si>
-  <si>
-    <t>1. Click burger menu icon</t>
-  </si>
-  <si>
-    <t>2. Click Close button</t>
-  </si>
-  <si>
-    <t>1. Click Cart icon</t>
-  </si>
-  <si>
-    <t>2. Click burger menu icon</t>
-  </si>
-  <si>
-    <t>3. Click Close button</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cart icon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> opens cart page</t>
-    </r>
-  </si>
-  <si>
-    <t>tbd</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Side nav</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> can be</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> closed</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> with close button on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inventory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page</t>
-    </r>
-  </si>
-  <si>
-    <t>Adding to cart</t>
-  </si>
-  <si>
-    <t>removing from cart</t>
-  </si>
-  <si>
-    <t>back to products link</t>
-  </si>
-  <si>
-    <r>
-      <t>Clicking</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> burger menu icon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> on the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> single item page</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> opens side nav bar which contains elements.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Side nav</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> can be </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>closed</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> with close button on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>single item page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>All items</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inventory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page redirects to inventory</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>About</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inventory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page redirects to about page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Logout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inventory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page logs out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Reset app state</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inventory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page resets app state</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>All items</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cart</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page redirects to inventory</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>About</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cart</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page redirects to about page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Logout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cart</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page logs out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Reset app state</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cart</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page resets app state</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>All items</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Single item</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page redirects to inventory</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>About</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Single item</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page redirects to about page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Reset app state</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Single item</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page resets app state</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Logout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Single item </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> page logs out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking each item's </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>image</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> opens a new page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking each item's </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>header</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> opens a new page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Add to cart </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>adds an item to cart</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Remove</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> removes the item from cart</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>twitter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> icon open twitter</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>facebook</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> cion open facebook </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Linkedin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> icon opens linkedin</t>
-    </r>
-  </si>
-  <si>
-    <t>default sorting in alphabetical asc</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">user can sort items in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>desc alphbtical</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> order</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">user can sort by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>price from low to high</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">user can sort by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>price from high to low</t>
-    </r>
-  </si>
-  <si>
-    <t>Error is displayed when trying to reach /inventory while not logged in</t>
-  </si>
-  <si>
-    <t>Error is displayed : 
-'Epic sadface: You can only access '/inventory.html' when you are logged in.'</t>
-  </si>
-  <si>
-    <t>Error is displayed when trying to reach /cart while not logged in</t>
-  </si>
-  <si>
-    <t>Error is displayed when trying to reach /checkout-step-one while not logged in</t>
-  </si>
-  <si>
-    <t>Error is displayed when trying to reach /inventory-item while not logged in</t>
-  </si>
-  <si>
-    <t>Error is displayed : 
-'Epic sadface: You can only access '/cart.html' when you are logged in.'</t>
-  </si>
-  <si>
-    <t>Error is displayed : 
-'Epic sadface: You can only access '/checkout-step-one.html' when you are logged in'</t>
-  </si>
-  <si>
-    <t>Error is displayed : 
-'Epic sadface: You can only access '/inventory-item.html' when you are logged in.'</t>
-  </si>
-  <si>
-    <t>1. Open https://www.saucedemo.com/cart.html</t>
-  </si>
-  <si>
-    <t>1. Open https://www.saucedemo.com/inventory-item.html?id=4</t>
-  </si>
-  <si>
-    <t>1. Open https://www.saucedemo.com/checkout-step-one.html</t>
-  </si>
-  <si>
-    <t>1. Open https://www.saucedemo.com/inventory.html</t>
   </si>
 </sst>
 </file>
@@ -2231,7 +2227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2357,11 +2353,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2382,15 +2381,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2402,17 +2401,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2697,9 +2696,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,10 +2725,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="45">
+      <c r="A2" s="46">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -2738,16 +2737,16 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="49"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2763,10 +2762,10 @@
       <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
+      <c r="A6" s="44">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="52" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -2775,16 +2774,16 @@
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
@@ -2800,10 +2799,10 @@
       <c r="E9" s="36"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
+      <c r="A10" s="44">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="52" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -2812,16 +2811,16 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="44"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
@@ -2837,10 +2836,10 @@
       <c r="E13" s="36"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
+      <c r="A14" s="44">
         <v>3</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="52" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -2849,16 +2848,16 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
@@ -2874,10 +2873,10 @@
       <c r="E17" s="36"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="43">
+      <c r="A18" s="44">
         <v>4</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="52" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -2886,16 +2885,16 @@
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="44"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="44"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
@@ -2911,10 +2910,10 @@
       <c r="E21" s="36"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
+      <c r="A22" s="44">
         <v>5</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="52" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -2923,16 +2922,16 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="44"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
@@ -2948,10 +2947,10 @@
       <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="43">
+      <c r="A26" s="44">
         <v>6</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="14" t="s">
@@ -2960,16 +2959,16 @@
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="44"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="44"/>
+      <c r="A28" s="44"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="3" t="s">
         <v>4</v>
       </c>
@@ -2985,10 +2984,10 @@
       <c r="E29" s="36"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="43">
+      <c r="A30" s="44">
         <v>7</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="45" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="14" t="s">
@@ -2997,16 +2996,16 @@
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
-      <c r="B31" s="51"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="51"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="3" t="s">
         <v>4</v>
       </c>
@@ -3015,16 +3014,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="51"/>
+      <c r="A33" s="44"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="51"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="3" t="s">
         <v>24</v>
       </c>
@@ -3033,16 +3032,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="51"/>
+      <c r="A35" s="44"/>
+      <c r="B35" s="45"/>
       <c r="C35" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="51"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="45"/>
       <c r="C36" s="3" t="s">
         <v>25</v>
       </c>
@@ -3051,16 +3050,16 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="51"/>
+      <c r="A37" s="44"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="51"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="45"/>
       <c r="C38" s="9" t="s">
         <v>26</v>
       </c>
@@ -3076,10 +3075,10 @@
       <c r="E39" s="36"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="43">
+      <c r="A40" s="44">
         <v>8</v>
       </c>
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="45" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="14" t="s">
@@ -3088,16 +3087,16 @@
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="51"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="45"/>
       <c r="C41" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="51"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="45"/>
       <c r="C42" s="9" t="s">
         <v>4</v>
       </c>
@@ -3113,10 +3112,10 @@
       <c r="E43" s="36"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="43">
+      <c r="A44" s="44">
         <v>9</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="45" t="s">
         <v>22</v>
       </c>
       <c r="C44" s="14" t="s">
@@ -3125,16 +3124,16 @@
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
-      <c r="B45" s="51"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
-      <c r="B46" s="51"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="45"/>
       <c r="C46" s="9" t="s">
         <v>4</v>
       </c>
@@ -3175,13 +3174,13 @@
         <v>11</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3196,13 +3195,13 @@
         <v>12</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3217,13 +3216,13 @@
         <v>13</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3238,13 +3237,13 @@
         <v>14</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3291,12 +3290,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A10:A12"/>
@@ -3305,12 +3304,12 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A30:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3321,9 +3320,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B2B3A2-C83E-447E-84CC-0452A4A8720F}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3344,7 +3343,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>41</v>
@@ -3356,41 +3355,36 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" s="53">
         <v>1</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>44</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>52</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="53"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="22"/>
+      <c r="B3" s="54"/>
+      <c r="D3" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="53"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="54"/>
+      <c r="D4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
     </row>
@@ -3406,14 +3400,14 @@
       <c r="A6" s="53">
         <v>2</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>63</v>
+      <c r="B6" s="54" t="s">
+        <v>61</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18" t="s">
@@ -3422,9 +3416,9 @@
     </row>
     <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
-      <c r="B7" s="52"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -3432,7 +3426,7 @@
     </row>
     <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
-      <c r="B8" s="52"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
@@ -3452,8 +3446,8 @@
       <c r="A10" s="53">
         <v>3</v>
       </c>
-      <c r="B10" s="52" t="s">
-        <v>83</v>
+      <c r="B10" s="54" t="s">
+        <v>81</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>44</v>
@@ -3465,9 +3459,9 @@
     </row>
     <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="53"/>
-      <c r="B11" s="52"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="18"/>
@@ -3475,7 +3469,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="53"/>
-      <c r="B12" s="52"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="22" t="s">
         <v>38</v>
       </c>
@@ -3495,29 +3489,29 @@
       <c r="A14" s="53">
         <v>4</v>
       </c>
-      <c r="B14" s="52" t="s">
-        <v>84</v>
+      <c r="B14" s="54" t="s">
+        <v>82</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="55"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="53"/>
-      <c r="B15" s="52"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="22"/>
       <c r="D15" s="18"/>
       <c r="E15" s="22"/>
-      <c r="F15" s="54"/>
+      <c r="F15" s="55"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="53"/>
-      <c r="B16" s="52"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="22"/>
       <c r="D16" s="18"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="54"/>
+      <c r="F16" s="55"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
@@ -3532,7 +3526,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3550,11 +3544,11 @@
       <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="55">
+      <c r="A22" s="56">
         <v>6</v>
       </c>
-      <c r="B22" s="52" t="s">
-        <v>86</v>
+      <c r="B22" s="54" t="s">
+        <v>84</v>
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -3562,16 +3556,16 @@
       <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="57"/>
-      <c r="B24" s="52"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="22"/>
       <c r="D24" s="25"/>
       <c r="E24" s="22"/>
@@ -3590,7 +3584,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -3610,7 +3604,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
@@ -3630,7 +3624,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
@@ -3650,7 +3644,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
@@ -3670,7 +3664,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
@@ -3690,7 +3684,7 @@
         <v>12</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
@@ -3710,7 +3704,7 @@
         <v>13</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
@@ -3974,18 +3968,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4018,7 +4012,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>41</v>
@@ -4034,39 +4028,39 @@
       <c r="A2" s="59">
         <v>1</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>54</v>
+      <c r="B2" s="55" t="s">
+        <v>52</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" s="22"/>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="55" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60"/>
-      <c r="B3" s="54"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="54"/>
+      <c r="F3" s="55"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="61"/>
-      <c r="B4" s="54"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="22"/>
-      <c r="F4" s="54"/>
+      <c r="F4" s="55"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
@@ -4080,14 +4074,14 @@
       <c r="A6" s="59">
         <v>2</v>
       </c>
-      <c r="B6" s="58" t="s">
-        <v>65</v>
+      <c r="B6" s="62" t="s">
+        <v>63</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>47</v>
@@ -4096,12 +4090,12 @@
     </row>
     <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
-      <c r="B7" s="54"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="22" t="s">
@@ -4110,7 +4104,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
-      <c r="B8" s="54"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
@@ -4130,39 +4124,39 @@
       <c r="A10" s="59">
         <v>3</v>
       </c>
-      <c r="B10" s="54" t="s">
-        <v>56</v>
+      <c r="B10" s="55" t="s">
+        <v>54</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E10" s="22"/>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="55" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
-      <c r="B11" s="54"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
-      <c r="B12" s="54"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="22"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="55"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -4176,14 +4170,14 @@
       <c r="A14" s="59">
         <v>4</v>
       </c>
-      <c r="B14" s="54" t="s">
-        <v>57</v>
+      <c r="B14" s="55" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>46</v>
@@ -4192,12 +4186,12 @@
     </row>
     <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
-      <c r="B15" s="54"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>47</v>
@@ -4206,12 +4200,12 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
-      <c r="B16" s="54"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22" t="s">
@@ -4230,17 +4224,17 @@
       <c r="A18" s="29">
         <v>5</v>
       </c>
-      <c r="B18" s="54" t="s">
-        <v>69</v>
+      <c r="B18" s="55" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="54"/>
+      <c r="B19" s="55"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
-      <c r="B20" s="54"/>
+      <c r="B20" s="55"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
@@ -4254,17 +4248,17 @@
       <c r="A22" s="29">
         <v>6</v>
       </c>
-      <c r="B22" s="54" t="s">
-        <v>70</v>
+      <c r="B22" s="55" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="54"/>
+      <c r="B23" s="55"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
@@ -4276,71 +4270,66 @@
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A2:A4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B6:B8"/>
@@ -4348,6 +4337,11 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4380,7 +4374,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>41</v>
@@ -4396,7 +4390,7 @@
       <c r="A2" s="53">
         <v>1</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -4408,9 +4402,9 @@
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="53"/>
-      <c r="B3" s="54"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -4418,7 +4412,7 @@
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
@@ -4504,7 +4498,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4513,19 +4507,19 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4632,7 +4626,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>41</v>
@@ -4648,7 +4642,7 @@
       <c r="A2" s="53">
         <v>1</v>
       </c>
-      <c r="B2" s="54"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -4656,7 +4650,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="53"/>
-      <c r="B3" s="54"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -4664,7 +4658,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>

</xml_diff>